<commit_message>
Updated Commands in DECODE UART
</commit_message>
<xml_diff>
--- a/manuals/DECODE UARTv2.xlsx
+++ b/manuals/DECODE UARTv2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\companion-module-dev\companion-module-lindy38152\manuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95435933-918A-46E0-8853-B3075DB5951F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF83241-5F55-429B-9431-CA943EE34AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4428" windowWidth="23256" windowHeight="13176" xr2:uid="{1E1C8624-581A-4565-B9A1-905C292B785E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E1C8624-581A-4565-B9A1-905C292B785E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2894" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3170" uniqueCount="121">
   <si>
     <t>A5</t>
   </si>
@@ -342,6 +342,63 @@
   </si>
   <si>
     <t>Set Default EDID to Input 1</t>
+  </si>
+  <si>
+    <t>Get Status Input1</t>
+  </si>
+  <si>
+    <t>Package1</t>
+  </si>
+  <si>
+    <t>Get Status Input2</t>
+  </si>
+  <si>
+    <t>Get Status Input3</t>
+  </si>
+  <si>
+    <t>Get Status Input4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Not connected</t>
+  </si>
+  <si>
+    <t>Get Status Output1</t>
+  </si>
+  <si>
+    <t>Get Status Output2</t>
+  </si>
+  <si>
+    <t>Get Status Output3</t>
+  </si>
+  <si>
+    <t>Get Status Output4</t>
+  </si>
+  <si>
+    <t>Connected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reply1 </t>
+  </si>
+  <si>
+    <t>Not connected</t>
+  </si>
+  <si>
+    <t>ENABLE BEEP</t>
+  </si>
+  <si>
+    <t>Set Ouptput 1 to input1</t>
+  </si>
+  <si>
+    <t>Set Output2 to input2</t>
+  </si>
+  <si>
+    <t>Set Output 3 to Input3</t>
+  </si>
+  <si>
+    <t>Set Output 4 to input4</t>
+  </si>
+  <si>
+    <t>AUDIO???</t>
   </si>
 </sst>
 </file>
@@ -357,7 +414,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +439,66 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -395,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -405,6 +522,16 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -739,20 +866,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6669995-09E3-4EFE-B614-260403C14034}">
-  <dimension ref="A1:Q312"/>
+  <dimension ref="A1:R348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T186" sqref="T186"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="22.90625" customWidth="1"/>
-    <col min="4" max="16" width="3.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="16" width="3.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="71" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="3" t="s">
         <v>34</v>
       </c>
@@ -773,7 +900,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>45</v>
       </c>
@@ -817,7 +944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -835,7 +962,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -845,19 +972,19 @@
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -878,8 +1005,11 @@
       <c r="P4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R4" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -889,19 +1019,19 @@
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -923,7 +1053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -933,19 +1063,19 @@
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="16" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -966,8 +1096,11 @@
       <c r="P6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R6" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -977,19 +1110,19 @@
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="16" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -1011,7 +1144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1021,19 +1154,19 @@
       <c r="E8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="F8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -1054,8 +1187,11 @@
       <c r="P8" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R8" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -1065,19 +1201,19 @@
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="16" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -1099,7 +1235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -1109,19 +1245,19 @@
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="F10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="16" t="s">
         <v>3</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="7" t="s">
         <v>3</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -1142,8 +1278,11 @@
       <c r="P10" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R10" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>28</v>
       </c>
@@ -1153,19 +1292,19 @@
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>4</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="K11" s="1" t="s">
@@ -1187,7 +1326,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>29</v>
       </c>
@@ -1197,10 +1336,10 @@
       <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>30</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -1230,8 +1369,11 @@
       <c r="P12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R12" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -1241,10 +1383,10 @@
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="F13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -1276,7 +1418,7 @@
       </c>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1286,10 +1428,10 @@
       <c r="E14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="F14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -1320,7 +1462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -1330,10 +1472,10 @@
       <c r="E15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="F15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -1364,7 +1506,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>39</v>
       </c>
@@ -1374,10 +1516,10 @@
       <c r="E16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -1407,8 +1549,11 @@
       <c r="P16" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R16" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>40</v>
       </c>
@@ -1418,10 +1563,10 @@
       <c r="E17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -1452,12 +1597,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -1467,10 +1612,10 @@
       <c r="E21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="F21" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>46</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -1479,7 +1624,7 @@
       <c r="I21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="10" t="s">
         <v>4</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -1501,7 +1646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -1511,10 +1656,10 @@
       <c r="E22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="F22" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="11" t="s">
         <v>46</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -1523,7 +1668,7 @@
       <c r="I22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="10" t="s">
         <v>13</v>
       </c>
       <c r="K22" s="1" t="s">
@@ -1545,12 +1690,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>21</v>
       </c>
@@ -1560,10 +1705,10 @@
       <c r="E26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -1594,7 +1739,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>20</v>
       </c>
@@ -1604,10 +1749,10 @@
       <c r="E27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -1638,12 +1783,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>21</v>
       </c>
@@ -1653,10 +1798,10 @@
       <c r="E30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -1687,7 +1832,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>20</v>
       </c>
@@ -1697,10 +1842,10 @@
       <c r="E31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -1731,12 +1876,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>21</v>
       </c>
@@ -1780,7 +1925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>18</v>
       </c>
@@ -1824,7 +1969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>22</v>
       </c>
@@ -1868,7 +2013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>19</v>
       </c>
@@ -1912,12 +2057,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>21</v>
       </c>
@@ -1961,7 +2106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>18</v>
       </c>
@@ -2005,7 +2150,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>22</v>
       </c>
@@ -2049,7 +2194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>19</v>
       </c>
@@ -2093,12 +2238,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>21</v>
       </c>
@@ -2142,7 +2287,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>18</v>
       </c>
@@ -2186,7 +2331,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>22</v>
       </c>
@@ -2230,7 +2375,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>19</v>
       </c>
@@ -2274,12 +2419,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>21</v>
       </c>
@@ -2323,7 +2468,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>18</v>
       </c>
@@ -2367,7 +2512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>22</v>
       </c>
@@ -2411,7 +2556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>19</v>
       </c>
@@ -2455,12 +2600,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>21</v>
       </c>
@@ -2504,7 +2649,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>18</v>
       </c>
@@ -2548,7 +2693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>22</v>
       </c>
@@ -2592,7 +2737,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>19</v>
       </c>
@@ -2636,12 +2781,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>21</v>
       </c>
@@ -2685,7 +2830,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>18</v>
       </c>
@@ -2729,7 +2874,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>22</v>
       </c>
@@ -2773,7 +2918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>19</v>
       </c>
@@ -2817,12 +2962,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>21</v>
       </c>
@@ -2866,7 +3011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>18</v>
       </c>
@@ -2910,12 +3055,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>21</v>
       </c>
@@ -2959,7 +3104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>18</v>
       </c>
@@ -3003,12 +3148,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>21</v>
       </c>
@@ -3052,7 +3197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>18</v>
       </c>
@@ -3096,12 +3241,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>21</v>
       </c>
@@ -3145,7 +3290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>18</v>
       </c>
@@ -3189,12 +3334,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>21</v>
       </c>
@@ -3238,7 +3383,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>18</v>
       </c>
@@ -3282,12 +3427,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>21</v>
       </c>
@@ -3331,7 +3476,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>18</v>
       </c>
@@ -3375,12 +3520,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>21</v>
       </c>
@@ -3424,7 +3569,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>18</v>
       </c>
@@ -3468,12 +3613,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>21</v>
       </c>
@@ -3517,7 +3662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>18</v>
       </c>
@@ -3561,12 +3706,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>21</v>
       </c>
@@ -3610,7 +3755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>18</v>
       </c>
@@ -3654,12 +3799,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>21</v>
       </c>
@@ -3703,7 +3848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>18</v>
       </c>
@@ -3747,12 +3892,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>21</v>
       </c>
@@ -3796,7 +3941,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>18</v>
       </c>
@@ -3840,12 +3985,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>21</v>
       </c>
@@ -3889,7 +4034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>18</v>
       </c>
@@ -3933,12 +4078,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>21</v>
       </c>
@@ -3982,7 +4127,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>18</v>
       </c>
@@ -4026,12 +4171,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>21</v>
       </c>
@@ -4075,7 +4220,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>18</v>
       </c>
@@ -4119,12 +4264,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>21</v>
       </c>
@@ -4168,7 +4313,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>18</v>
       </c>
@@ -4212,12 +4357,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>21</v>
       </c>
@@ -4261,7 +4406,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>18</v>
       </c>
@@ -4305,12 +4450,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>21</v>
       </c>
@@ -4354,7 +4499,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>18</v>
       </c>
@@ -4398,7 +4543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>22</v>
       </c>
@@ -4442,7 +4587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>19</v>
       </c>
@@ -4486,7 +4631,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>24</v>
       </c>
@@ -4530,7 +4675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>74</v>
       </c>
@@ -4574,7 +4719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>76</v>
       </c>
@@ -4618,17 +4763,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>21</v>
       </c>
@@ -4672,7 +4817,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>18</v>
       </c>
@@ -4716,7 +4861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>22</v>
       </c>
@@ -4760,7 +4905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>19</v>
       </c>
@@ -4804,7 +4949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>24</v>
       </c>
@@ -4848,7 +4993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>74</v>
       </c>
@@ -4892,7 +5037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>76</v>
       </c>
@@ -4936,17 +5081,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>21</v>
       </c>
@@ -4990,7 +5135,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>18</v>
       </c>
@@ -5034,7 +5179,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>22</v>
       </c>
@@ -5078,7 +5223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>19</v>
       </c>
@@ -5122,7 +5267,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>24</v>
       </c>
@@ -5166,7 +5311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>74</v>
       </c>
@@ -5210,7 +5355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>76</v>
       </c>
@@ -5254,17 +5399,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>21</v>
       </c>
@@ -5308,7 +5453,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>18</v>
       </c>
@@ -5352,7 +5497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>22</v>
       </c>
@@ -5396,7 +5541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>19</v>
       </c>
@@ -5440,7 +5585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>24</v>
       </c>
@@ -5484,7 +5629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>74</v>
       </c>
@@ -5528,7 +5673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>76</v>
       </c>
@@ -5572,17 +5717,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>21</v>
       </c>
@@ -5626,7 +5771,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>18</v>
       </c>
@@ -5670,7 +5815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>22</v>
       </c>
@@ -5714,7 +5859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>19</v>
       </c>
@@ -5758,7 +5903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>24</v>
       </c>
@@ -5802,7 +5947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>74</v>
       </c>
@@ -5846,7 +5991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>76</v>
       </c>
@@ -5890,17 +6035,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>21</v>
       </c>
@@ -5944,7 +6089,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>18</v>
       </c>
@@ -5988,7 +6133,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>22</v>
       </c>
@@ -6032,7 +6177,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>19</v>
       </c>
@@ -6076,7 +6221,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>24</v>
       </c>
@@ -6120,7 +6265,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>74</v>
       </c>
@@ -6164,7 +6309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>76</v>
       </c>
@@ -6208,17 +6353,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>21</v>
       </c>
@@ -6262,7 +6407,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>18</v>
       </c>
@@ -6306,7 +6451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>22</v>
       </c>
@@ -6350,7 +6495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>19</v>
       </c>
@@ -6394,7 +6539,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>24</v>
       </c>
@@ -6438,7 +6583,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>74</v>
       </c>
@@ -6482,7 +6627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>76</v>
       </c>
@@ -6526,17 +6671,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>21</v>
       </c>
@@ -6580,7 +6725,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>18</v>
       </c>
@@ -6624,7 +6769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>22</v>
       </c>
@@ -6668,7 +6813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>19</v>
       </c>
@@ -6712,7 +6857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>24</v>
       </c>
@@ -6756,7 +6901,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
         <v>74</v>
       </c>
@@ -6800,7 +6945,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>76</v>
       </c>
@@ -6844,17 +6989,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
         <v>21</v>
       </c>
@@ -6898,7 +7043,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
         <v>18</v>
       </c>
@@ -6942,7 +7087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>22</v>
       </c>
@@ -6986,7 +7131,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
         <v>19</v>
       </c>
@@ -7030,7 +7175,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
         <v>24</v>
       </c>
@@ -7074,7 +7219,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
         <v>74</v>
       </c>
@@ -7118,7 +7263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
         <v>76</v>
       </c>
@@ -7162,17 +7307,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
         <v>21</v>
       </c>
@@ -7216,7 +7361,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
         <v>18</v>
       </c>
@@ -7260,7 +7405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
         <v>22</v>
       </c>
@@ -7304,7 +7449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
         <v>19</v>
       </c>
@@ -7348,7 +7493,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
         <v>24</v>
       </c>
@@ -7392,7 +7537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
         <v>74</v>
       </c>
@@ -7436,7 +7581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
         <v>76</v>
       </c>
@@ -7480,17 +7625,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
         <v>21</v>
       </c>
@@ -7534,7 +7679,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
         <v>18</v>
       </c>
@@ -7578,7 +7723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
         <v>22</v>
       </c>
@@ -7622,7 +7767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
         <v>19</v>
       </c>
@@ -7666,7 +7811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
         <v>24</v>
       </c>
@@ -7710,7 +7855,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
         <v>74</v>
       </c>
@@ -7754,7 +7899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
         <v>76</v>
       </c>
@@ -7798,17 +7943,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
         <v>21</v>
       </c>
@@ -7852,7 +7997,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
         <v>18</v>
       </c>
@@ -7896,7 +8041,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
         <v>22</v>
       </c>
@@ -7940,7 +8085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
         <v>19</v>
       </c>
@@ -7984,7 +8129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
         <v>24</v>
       </c>
@@ -8028,7 +8173,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
         <v>74</v>
       </c>
@@ -8072,7 +8217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
         <v>76</v>
       </c>
@@ -8116,17 +8261,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
         <v>21</v>
       </c>
@@ -8170,7 +8315,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
         <v>18</v>
       </c>
@@ -8214,7 +8359,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
         <v>22</v>
       </c>
@@ -8258,7 +8403,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
         <v>19</v>
       </c>
@@ -8302,7 +8447,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
         <v>24</v>
       </c>
@@ -8346,7 +8491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
         <v>74</v>
       </c>
@@ -8390,7 +8535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
         <v>76</v>
       </c>
@@ -8434,17 +8579,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
         <v>21</v>
       </c>
@@ -8488,7 +8633,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
         <v>18</v>
       </c>
@@ -8532,7 +8677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
         <v>22</v>
       </c>
@@ -8576,7 +8721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
         <v>19</v>
       </c>
@@ -8620,7 +8765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
         <v>24</v>
       </c>
@@ -8664,7 +8809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
         <v>74</v>
       </c>
@@ -8708,7 +8853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
         <v>76</v>
       </c>
@@ -8752,17 +8897,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="274" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
         <v>21</v>
       </c>
@@ -8806,7 +8951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
         <v>18</v>
       </c>
@@ -8850,7 +8995,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="277" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
         <v>22</v>
       </c>
@@ -8894,7 +9039,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
         <v>19</v>
       </c>
@@ -8938,7 +9083,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="279" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
         <v>24</v>
       </c>
@@ -8982,7 +9127,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="280" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
         <v>74</v>
       </c>
@@ -9026,7 +9171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="281" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
         <v>76</v>
       </c>
@@ -9070,17 +9215,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="282" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="284" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="285" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
         <v>21</v>
       </c>
@@ -9124,7 +9269,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
         <v>18</v>
       </c>
@@ -9168,7 +9313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
         <v>22</v>
       </c>
@@ -9212,7 +9357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
         <v>19</v>
       </c>
@@ -9256,7 +9401,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
         <v>24</v>
       </c>
@@ -9300,7 +9445,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
         <v>74</v>
       </c>
@@ -9344,7 +9489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
         <v>76</v>
       </c>
@@ -9388,17 +9533,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
         <v>21</v>
       </c>
@@ -9442,7 +9587,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
         <v>18</v>
       </c>
@@ -9486,7 +9631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
         <v>22</v>
       </c>
@@ -9530,7 +9675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
         <v>19</v>
       </c>
@@ -9574,7 +9719,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
         <v>24</v>
       </c>
@@ -9618,7 +9763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="300" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
         <v>74</v>
       </c>
@@ -9662,7 +9807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
         <v>76</v>
       </c>
@@ -9675,7 +9820,7 @@
       <c r="F301" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G301" s="1" t="s">
+      <c r="G301" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H301" s="4" t="s">
@@ -9706,17 +9851,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="305" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
         <v>21</v>
       </c>
@@ -9760,7 +9905,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="306" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
         <v>18</v>
       </c>
@@ -9804,7 +9949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="307" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
         <v>22</v>
       </c>
@@ -9848,7 +9993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="308" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
         <v>19</v>
       </c>
@@ -9892,7 +10037,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="309" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
         <v>24</v>
       </c>
@@ -9936,7 +10081,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="310" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
         <v>74</v>
       </c>
@@ -9980,7 +10125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="311" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
         <v>76</v>
       </c>
@@ -9993,7 +10138,7 @@
       <c r="F311" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G311" s="1" t="s">
+      <c r="G311" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H311" s="4" t="s">
@@ -10024,9 +10169,911 @@
         <v>50</v>
       </c>
     </row>
-    <row r="312" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="316" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="317" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B317" t="s">
+        <v>103</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F317" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G317" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H317" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I317" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J317" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K317" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L317" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M317" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N317" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O317" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P317" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="318" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B318" t="s">
+        <v>18</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F318" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G318" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H318" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I318" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J318" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K318" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L318" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M318" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N318" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O318" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P318" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q318" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="319" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B319" t="s">
+        <v>113</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F319" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G319" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H319" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I319" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J319" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K319" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L319" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M319" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N319" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O319" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P319" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q319" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="320" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F320" s="9"/>
+      <c r="G320" s="12"/>
+    </row>
+    <row r="321" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>104</v>
+      </c>
+      <c r="F321" s="9"/>
+      <c r="G321" s="12"/>
+    </row>
+    <row r="322" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B322" t="s">
+        <v>103</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E322" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F322" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G322" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H322" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I322" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J322" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K322" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L322" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M322" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N322" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O322" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P322" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="323" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B323" t="s">
+        <v>18</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E323" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F323" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G323" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H323" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I323" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J323" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K323" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L323" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M323" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N323" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O323" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P323" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q323" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="324" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F324" s="9"/>
+      <c r="G324" s="12"/>
+    </row>
+    <row r="325" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>105</v>
+      </c>
+      <c r="F325" s="9"/>
+      <c r="G325" s="12"/>
+    </row>
+    <row r="326" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B326" t="s">
+        <v>103</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E326" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F326" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G326" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H326" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I326" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J326" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K326" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L326" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M326" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N326" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O326" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P326" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="327" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B327" t="s">
+        <v>18</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E327" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F327" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G327" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H327" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I327" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J327" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K327" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L327" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M327" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N327" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O327" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P327" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q327" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="328" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F328" s="9"/>
+      <c r="G328" s="12"/>
+    </row>
+    <row r="329" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>106</v>
+      </c>
+      <c r="F329" s="9"/>
+      <c r="G329" s="12"/>
+    </row>
+    <row r="330" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B330" t="s">
+        <v>103</v>
+      </c>
+      <c r="D330" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F330" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G330" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H330" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I330" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J330" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K330" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L330" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M330" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N330" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O330" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P330" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="331" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B331" t="s">
+        <v>18</v>
+      </c>
+      <c r="D331" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E331" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F331" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G331" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H331" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I331" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J331" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K331" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L331" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M331" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N331" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O331" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P331" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q331" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="332" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F332" s="9"/>
+    </row>
+    <row r="333" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>108</v>
+      </c>
+      <c r="F333" s="9"/>
+    </row>
+    <row r="334" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B334" t="s">
+        <v>103</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F334" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G334" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H334" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I334" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J334" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K334" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L334" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M334" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N334" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O334" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P334" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="335" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B335" t="s">
+        <v>18</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E335" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F335" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G335" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H335" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I335" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J335" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K335" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L335" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M335" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N335" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O335" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P335" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q335" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="336" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B336" t="s">
+        <v>18</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E336" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F336" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G336" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H336" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I336" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J336" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K336" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L336" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M336" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N336" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O336" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P336" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q336" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="337" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F337" s="9"/>
+      <c r="G337" s="4"/>
+    </row>
+    <row r="338" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>109</v>
+      </c>
+      <c r="F338" s="9"/>
+      <c r="G338" s="4"/>
+    </row>
+    <row r="339" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B339" t="s">
+        <v>103</v>
+      </c>
+      <c r="D339" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F339" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G339" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H339" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I339" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J339" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K339" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L339" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M339" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N339" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O339" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P339" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="340" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B340" t="s">
+        <v>18</v>
+      </c>
+      <c r="D340" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E340" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F340" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G340" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H340" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I340" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J340" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K340" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L340" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M340" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N340" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O340" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P340" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q340" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="341" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F341" s="9"/>
+      <c r="G341" s="4"/>
+    </row>
+    <row r="342" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>110</v>
+      </c>
+      <c r="F342" s="9"/>
+      <c r="G342" s="4"/>
+    </row>
+    <row r="343" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B343" t="s">
+        <v>103</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E343" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F343" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G343" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H343" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I343" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J343" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K343" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L343" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M343" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N343" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O343" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P343" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="344" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B344" t="s">
+        <v>18</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E344" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F344" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G344" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H344" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I344" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J344" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K344" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L344" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M344" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N344" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O344" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P344" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q344" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="345" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F345" s="9"/>
+      <c r="G345" s="4"/>
+    </row>
+    <row r="346" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>111</v>
+      </c>
+      <c r="F346" s="9"/>
+      <c r="G346" s="4"/>
+    </row>
+    <row r="347" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B347" t="s">
+        <v>103</v>
+      </c>
+      <c r="D347" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E347" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F347" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G347" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H347" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I347" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J347" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K347" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L347" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M347" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N347" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O347" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P347" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="348" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B348" t="s">
+        <v>18</v>
+      </c>
+      <c r="D348" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E348" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F348" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G348" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H348" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I348" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J348" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K348" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L348" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M348" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N348" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O348" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P348" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q348" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report status to Server to Show in GUI
</commit_message>
<xml_diff>
--- a/manuals/DECODE UARTv2.xlsx
+++ b/manuals/DECODE UARTv2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\companion-module-dev\companion-module-lindy38152\manuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF83241-5F55-429B-9431-CA943EE34AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A232DC-E585-4655-94E8-B3BE5D3EB9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E1C8624-581A-4565-B9A1-905C292B785E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
+    <sheet name="RAWData" sheetId="2" r:id="rId1"/>
+    <sheet name="Bytes" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3170" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3316" uniqueCount="147">
   <si>
     <t>A5</t>
   </si>
@@ -399,6 +400,84 @@
   </si>
   <si>
     <t>AUDIO???</t>
+  </si>
+  <si>
+    <t>01 [Status]</t>
+  </si>
+  <si>
+    <t>[Command]</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>01-04 [Channel]</t>
+  </si>
+  <si>
+    <t>Status request</t>
+  </si>
+  <si>
+    <t>Status reply</t>
+  </si>
+  <si>
+    <t>00[Connected]/ FF [Not Connected]</t>
+  </si>
+  <si>
+    <t>04 [Input] / 05[Output]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connect </t>
+  </si>
+  <si>
+    <t>Connect Reply</t>
+  </si>
+  <si>
+    <t>0B [Device itself]</t>
+  </si>
+  <si>
+    <t>BYTE -&gt;</t>
+  </si>
+  <si>
+    <t>RS232 Command</t>
+  </si>
+  <si>
+    <t>FF [online] (No answer when Offline)??</t>
+  </si>
+  <si>
+    <t>06 [Beep]</t>
+  </si>
+  <si>
+    <t>F0 [deactivate]</t>
+  </si>
+  <si>
+    <t>0F [activate]</t>
+  </si>
+  <si>
+    <t>Disable Beep Reply</t>
+  </si>
+  <si>
+    <t>Enable Beep Reply</t>
+  </si>
+  <si>
+    <t>Set Out to IN</t>
+  </si>
+  <si>
+    <t>02 [SetOut]</t>
+  </si>
+  <si>
+    <t>03 [SetOut]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00 </t>
+  </si>
+  <si>
+    <t>Reply Out to IN</t>
+  </si>
+  <si>
+    <t>00-04 [output Number]</t>
+  </si>
+  <si>
+    <t>01-04 [input number]</t>
   </si>
 </sst>
 </file>
@@ -868,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6669995-09E3-4EFE-B614-260403C14034}">
   <dimension ref="A1:R348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="T305" sqref="T305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4732,7 +4811,7 @@
       <c r="F141" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G141" s="1" t="s">
+      <c r="G141" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H141" s="4" t="s">
@@ -5050,7 +5129,7 @@
       <c r="F151" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G151" s="1" t="s">
+      <c r="G151" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H151" s="4" t="s">
@@ -5368,7 +5447,7 @@
       <c r="F161" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G161" s="1" t="s">
+      <c r="G161" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H161" s="4" t="s">
@@ -5686,7 +5765,7 @@
       <c r="F171" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G171" s="1" t="s">
+      <c r="G171" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H171" s="4" t="s">
@@ -6004,7 +6083,7 @@
       <c r="F181" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G181" s="1" t="s">
+      <c r="G181" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H181" s="4" t="s">
@@ -6322,7 +6401,7 @@
       <c r="F191" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G191" s="1" t="s">
+      <c r="G191" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H191" s="4" t="s">
@@ -6640,7 +6719,7 @@
       <c r="F201" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G201" s="1" t="s">
+      <c r="G201" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H201" s="4" t="s">
@@ -6958,7 +7037,7 @@
       <c r="F211" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G211" s="1" t="s">
+      <c r="G211" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H211" s="4" t="s">
@@ -7276,7 +7355,7 @@
       <c r="F221" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G221" s="1" t="s">
+      <c r="G221" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H221" s="4" t="s">
@@ -7594,7 +7673,7 @@
       <c r="F231" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G231" s="1" t="s">
+      <c r="G231" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H231" s="4" t="s">
@@ -7912,7 +7991,7 @@
       <c r="F241" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G241" s="1" t="s">
+      <c r="G241" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H241" s="4" t="s">
@@ -8230,7 +8309,7 @@
       <c r="F251" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G251" s="1" t="s">
+      <c r="G251" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H251" s="4" t="s">
@@ -8548,7 +8627,7 @@
       <c r="F261" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G261" s="1" t="s">
+      <c r="G261" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H261" s="4" t="s">
@@ -8866,7 +8945,7 @@
       <c r="F271" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G271" s="1" t="s">
+      <c r="G271" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H271" s="4" t="s">
@@ -9184,7 +9263,7 @@
       <c r="F281" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G281" s="1" t="s">
+      <c r="G281" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H281" s="4" t="s">
@@ -9502,7 +9581,7 @@
       <c r="F291" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G291" s="1" t="s">
+      <c r="G291" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H291" s="4" t="s">
@@ -11074,6 +11153,554 @@
       </c>
       <c r="Q348" s="1" t="s">
         <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2176F797-D6C5-4E12-89B5-8FED5F5DA648}">
+  <dimension ref="A2:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="3" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1"/>
+    <col min="9" max="14" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2">
+        <v>9</v>
+      </c>
+      <c r="K3" s="2">
+        <v>10</v>
+      </c>
+      <c r="L3" s="2">
+        <v>11</v>
+      </c>
+      <c r="M3" s="2">
+        <v>12</v>
+      </c>
+      <c r="N3" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>